<commit_message>
add tag support for urllist uploads and downloads
</commit_message>
<xml_diff>
--- a/tests/test spreadsheet uploads/waterschappen.xlsx
+++ b/tests/test spreadsheet uploads/waterschappen.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="31">
   <si>
     <t xml:space="preserve">Category / List</t>
   </si>
@@ -28,12 +28,18 @@
     <t xml:space="preserve">Website</t>
   </si>
   <si>
+    <t xml:space="preserve">Tags</t>
+  </si>
+  <si>
     <t xml:space="preserve">waterschappen, testsites</t>
   </si>
   <si>
     <t xml:space="preserve">aaenmaas.nl</t>
   </si>
   <si>
+    <t xml:space="preserve">test</t>
+  </si>
+  <si>
     <t xml:space="preserve">waterschappen</t>
   </si>
   <si>
@@ -49,6 +55,9 @@
     <t xml:space="preserve">dommel.nl</t>
   </si>
   <si>
+    <t xml:space="preserve">waterschap</t>
+  </si>
+  <si>
     <t xml:space="preserve">hhdelfland.nl</t>
   </si>
   <si>
@@ -85,6 +94,9 @@
     <t xml:space="preserve">hdsr.nl</t>
   </si>
   <si>
+    <t xml:space="preserve">test, waterschap, extra</t>
+  </si>
+  <si>
     <t xml:space="preserve">vallei-veluwe.nl</t>
   </si>
   <si>
@@ -98,6 +110,9 @@
   </si>
   <si>
     <t xml:space="preserve">zuiderzeeland.nl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">extra</t>
   </si>
 </sst>
 </file>
@@ -113,6 +128,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -128,6 +144,65 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFCC0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <i val="true"/>
+      <sz val="10"/>
+      <color rgb="FF808080"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF006600"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -135,82 +210,36 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="18"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <u val="single"/>
+      <sz val="10"/>
+      <color rgb="FF0000EE"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF996600"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF333333"/>
       <name val="Arial"/>
       <family val="2"/>
-    </font>
-    <font>
-      <i val="true"/>
-      <sz val="10"/>
-      <color rgb="FF808080"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <u val="single"/>
-      <sz val="10"/>
-      <color rgb="FF0000EE"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF006600"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF996600"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FFCC0000"/>
-      <name val="Arial"/>
-      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
       <sz val="10"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="9">
@@ -222,8 +251,32 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor rgb="FFFFFFFF"/>
+        <fgColor rgb="FF000000"/>
+        <bgColor rgb="FF003300"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF808080"/>
+        <bgColor rgb="FF969696"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDDDDDD"/>
+        <bgColor rgb="FFFFCCCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCCCC"/>
+        <bgColor rgb="FFDDDDDD"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCC0000"/>
+        <bgColor rgb="FF800000"/>
       </patternFill>
     </fill>
     <fill>
@@ -234,32 +287,8 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCCCC"/>
-        <bgColor rgb="FFDDDDDD"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFCC0000"/>
-        <bgColor rgb="FF800000"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF000000"/>
-        <bgColor rgb="FF003300"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF808080"/>
-        <bgColor rgb="FF969696"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFDDDDDD"/>
-        <bgColor rgb="FFFFCCCC"/>
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
   </fills>
@@ -326,30 +355,64 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="1" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="10" fillId="3" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="11" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="12" fillId="4" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="13" fillId="5" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="15" fillId="6" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="15" fillId="7" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="14" fillId="8" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="4" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="5" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="6" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="7" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="8" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="8" borderId="1" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="16" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -369,23 +432,23 @@
     <cellStyle name="Currency" xfId="17" builtinId="4"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
-    <cellStyle name="Heading" xfId="20"/>
-    <cellStyle name="Heading 1" xfId="21"/>
-    <cellStyle name="Heading 2" xfId="22"/>
-    <cellStyle name="Text" xfId="23"/>
-    <cellStyle name="Note" xfId="24"/>
-    <cellStyle name="Footnote" xfId="25"/>
-    <cellStyle name="Hyperlink" xfId="26"/>
-    <cellStyle name="Status" xfId="27"/>
-    <cellStyle name="Good" xfId="28"/>
-    <cellStyle name="Neutral" xfId="29"/>
-    <cellStyle name="Bad" xfId="30"/>
-    <cellStyle name="Warning" xfId="31"/>
-    <cellStyle name="Error" xfId="32"/>
-    <cellStyle name="Accent" xfId="33"/>
-    <cellStyle name="Accent 1" xfId="34"/>
-    <cellStyle name="Accent 2" xfId="35"/>
-    <cellStyle name="Accent 3" xfId="36"/>
+    <cellStyle name="Accent 1 17" xfId="20"/>
+    <cellStyle name="Accent 16" xfId="21"/>
+    <cellStyle name="Accent 2 18" xfId="22"/>
+    <cellStyle name="Accent 3 19" xfId="23"/>
+    <cellStyle name="Bad 13" xfId="24"/>
+    <cellStyle name="Error 15" xfId="25"/>
+    <cellStyle name="Footnote 8" xfId="26"/>
+    <cellStyle name="Good 11" xfId="27"/>
+    <cellStyle name="Heading 1 4" xfId="28"/>
+    <cellStyle name="Heading 2 5" xfId="29"/>
+    <cellStyle name="Heading 3" xfId="30"/>
+    <cellStyle name="Hyperlink 9" xfId="31"/>
+    <cellStyle name="Neutral 12" xfId="32"/>
+    <cellStyle name="Note 7" xfId="33"/>
+    <cellStyle name="Status 10" xfId="34"/>
+    <cellStyle name="Text 6" xfId="35"/>
+    <cellStyle name="Warning 14" xfId="36"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -451,21 +514,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B26"/>
+  <dimension ref="A1:C26"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="76" zoomScaleNormal="76" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="26.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="30.01"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="30.02"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="17.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -475,181 +537,223 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="0" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>8</v>
+        <v>10</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>9</v>
+        <v>12</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>12</v>
+        <v>15</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>13</v>
+        <v>16</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>16</v>
+        <v>19</v>
+      </c>
+      <c r="C14" s="0" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>17</v>
+        <v>20</v>
+      </c>
+      <c r="C15" s="0" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>20</v>
+        <v>23</v>
+      </c>
+      <c r="C18" s="0" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>21</v>
+        <v>25</v>
+      </c>
+      <c r="C19" s="0" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>22</v>
+        <v>26</v>
+      </c>
+      <c r="C20" s="0" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>23</v>
+        <v>27</v>
+      </c>
+      <c r="C21" s="0" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>25</v>
+        <v>29</v>
+      </c>
+      <c r="C23" s="0" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -664,7 +768,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>

</xml_diff>